<commit_message>
bugfix: fix generator.py and update results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nggeo\Desktop\4211-PAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BEB9BF-8BE6-42F1-82C9-90F090611A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3891911-B898-4836-BC86-5172AD1C4C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5505" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,7 +422,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,8 +602,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -718,6 +724,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -767,7 +788,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1127,7 +1148,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D2" sqref="D2:E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,18 +1212,18 @@
         <v>2</v>
       </c>
       <c r="D2" s="2">
-        <v>0.32707999999999998</v>
+        <v>0.30052000000000001</v>
       </c>
       <c r="E2" s="2">
-        <v>0.58572999999999997</v>
+        <v>0.64097000000000004</v>
       </c>
       <c r="F2">
         <f>1-E2</f>
-        <v>0.41427000000000003</v>
+        <v>0.35902999999999996</v>
       </c>
       <c r="G2">
         <f>1-D2</f>
-        <v>0.67291999999999996</v>
+        <v>0.69947999999999999</v>
       </c>
       <c r="H2">
         <f>IF(E2&gt;G2,1,2)</f>
@@ -1214,11 +1235,11 @@
       </c>
       <c r="J2" s="1">
         <f>ABS(G2-E2)</f>
-        <v>8.718999999999999E-2</v>
+        <v>5.8509999999999951E-2</v>
       </c>
       <c r="K2" s="1">
         <f>SUM(I:I)/100</f>
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1232,18 +1253,18 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>0.35236000000000001</v>
+        <v>0.34531000000000001</v>
       </c>
       <c r="E3" s="2">
-        <v>0.62663999999999997</v>
+        <v>0.62797000000000003</v>
       </c>
       <c r="F3">
         <f>1-E3</f>
-        <v>0.37336000000000003</v>
+        <v>0.37202999999999997</v>
       </c>
       <c r="G3">
         <f>1-D3</f>
-        <v>0.64763999999999999</v>
+        <v>0.65468999999999999</v>
       </c>
       <c r="H3">
         <f>IF(E3&gt;G3,1,2)</f>
@@ -1255,7 +1276,7 @@
       </c>
       <c r="J3" s="1">
         <f>ABS(G3-E3)</f>
-        <v>2.1000000000000019E-2</v>
+        <v>2.6719999999999966E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1269,18 +1290,18 @@
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>0.27109</v>
+        <v>0.31707999999999997</v>
       </c>
       <c r="E4" s="2">
-        <v>0.60958999999999997</v>
+        <v>0.66815999999999998</v>
       </c>
       <c r="F4">
         <f>1-E4</f>
-        <v>0.39041000000000003</v>
+        <v>0.33184000000000002</v>
       </c>
       <c r="G4">
         <f>1-D4</f>
-        <v>0.72890999999999995</v>
+        <v>0.68291999999999997</v>
       </c>
       <c r="H4">
         <f>IF(E4&gt;G4,1,2)</f>
@@ -1292,7 +1313,7 @@
       </c>
       <c r="J4" s="1">
         <f>ABS(G4-E4)</f>
-        <v>0.11931999999999998</v>
+        <v>1.4759999999999995E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1306,18 +1327,18 @@
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>0.32501999999999998</v>
+        <v>0.31245000000000001</v>
       </c>
       <c r="E5" s="2">
-        <v>0.56672</v>
+        <v>0.62163000000000002</v>
       </c>
       <c r="F5">
         <f>1-E5</f>
-        <v>0.43328</v>
+        <v>0.37836999999999998</v>
       </c>
       <c r="G5">
         <f>1-D5</f>
-        <v>0.67498000000000002</v>
+        <v>0.68754999999999999</v>
       </c>
       <c r="H5">
         <f>IF(E5&gt;G5,1,2)</f>
@@ -1329,7 +1350,7 @@
       </c>
       <c r="J5" s="1">
         <f>ABS(G5-E5)</f>
-        <v>0.10826000000000002</v>
+        <v>6.5919999999999979E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1343,18 +1364,18 @@
         <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>0.39129999999999998</v>
+        <v>0.39616000000000001</v>
       </c>
       <c r="E6" s="2">
-        <v>0.64219000000000004</v>
+        <v>0.66735999999999995</v>
       </c>
       <c r="F6">
         <f>1-E6</f>
-        <v>0.35780999999999996</v>
+        <v>0.33264000000000005</v>
       </c>
       <c r="G6">
         <f>1-D6</f>
-        <v>0.60870000000000002</v>
+        <v>0.60383999999999993</v>
       </c>
       <c r="H6">
         <f>IF(E6&gt;G6,1,2)</f>
@@ -1366,7 +1387,7 @@
       </c>
       <c r="J6" s="1">
         <f>ABS(G6-E6)</f>
-        <v>3.349000000000002E-2</v>
+        <v>6.3520000000000021E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1380,18 +1401,18 @@
         <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>0.42971999999999999</v>
+        <v>0.42120000000000002</v>
       </c>
       <c r="E7" s="2">
-        <v>0.61234999999999995</v>
+        <v>0.64361000000000002</v>
       </c>
       <c r="F7">
         <f>1-E7</f>
-        <v>0.38765000000000005</v>
+        <v>0.35638999999999998</v>
       </c>
       <c r="G7">
         <f>1-D7</f>
-        <v>0.57028000000000001</v>
+        <v>0.57879999999999998</v>
       </c>
       <c r="H7">
         <f>IF(E7&gt;G7,1,2)</f>
@@ -1403,7 +1424,7 @@
       </c>
       <c r="J7" s="1">
         <f>ABS(G7-E7)</f>
-        <v>4.2069999999999941E-2</v>
+        <v>6.4810000000000034E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1417,18 +1438,18 @@
         <v>2</v>
       </c>
       <c r="D8" s="2">
-        <v>0.20344999999999999</v>
+        <v>0.1978</v>
       </c>
       <c r="E8" s="2">
-        <v>0.64990000000000003</v>
+        <v>0.66820000000000002</v>
       </c>
       <c r="F8">
         <f>1-E8</f>
-        <v>0.35009999999999997</v>
+        <v>0.33179999999999998</v>
       </c>
       <c r="G8">
         <f>1-D8</f>
-        <v>0.79654999999999998</v>
+        <v>0.80220000000000002</v>
       </c>
       <c r="H8">
         <f>IF(E8&gt;G8,1,2)</f>
@@ -1440,7 +1461,7 @@
       </c>
       <c r="J8" s="1">
         <f>ABS(G8-E8)</f>
-        <v>0.14664999999999995</v>
+        <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1454,18 +1475,18 @@
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>0.27847</v>
+        <v>0.30603000000000002</v>
       </c>
       <c r="E9" s="2">
-        <v>0.62795999999999996</v>
+        <v>0.62680999999999998</v>
       </c>
       <c r="F9">
         <f>1-E9</f>
-        <v>0.37204000000000004</v>
+        <v>0.37319000000000002</v>
       </c>
       <c r="G9">
         <f>1-D9</f>
-        <v>0.72153</v>
+        <v>0.69396999999999998</v>
       </c>
       <c r="H9">
         <f>IF(E9&gt;G9,1,2)</f>
@@ -1477,7 +1498,7 @@
       </c>
       <c r="J9" s="1">
         <f>ABS(G9-E9)</f>
-        <v>9.3570000000000042E-2</v>
+        <v>6.7159999999999997E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1491,30 +1512,30 @@
         <v>2</v>
       </c>
       <c r="D10" s="2">
-        <v>0.35178999999999999</v>
+        <v>0.39854000000000001</v>
       </c>
       <c r="E10" s="2">
-        <v>0.59306000000000003</v>
+        <v>0.64210999999999996</v>
       </c>
       <c r="F10">
         <f>1-E10</f>
-        <v>0.40693999999999997</v>
+        <v>0.35789000000000004</v>
       </c>
       <c r="G10">
         <f>1-D10</f>
-        <v>0.64820999999999995</v>
+        <v>0.60145999999999999</v>
       </c>
       <c r="H10">
         <f>IF(E10&gt;G10,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f>IF(H10=C10,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1">
         <f>ABS(G10-E10)</f>
-        <v>5.5149999999999921E-2</v>
+        <v>4.0649999999999964E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1528,18 +1549,18 @@
         <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>0.23810999999999999</v>
+        <v>0.20885999999999999</v>
       </c>
       <c r="E11" s="2">
-        <v>0.64978000000000002</v>
+        <v>0.71536</v>
       </c>
       <c r="F11">
         <f>1-E11</f>
-        <v>0.35021999999999998</v>
+        <v>0.28464</v>
       </c>
       <c r="G11">
         <f>1-D11</f>
-        <v>0.76188999999999996</v>
+        <v>0.79113999999999995</v>
       </c>
       <c r="H11">
         <f>IF(E11&gt;G11,1,2)</f>
@@ -1551,7 +1572,7 @@
       </c>
       <c r="J11" s="1">
         <f>ABS(G11-E11)</f>
-        <v>0.11210999999999993</v>
+        <v>7.5779999999999959E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1565,18 +1586,18 @@
         <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0.38501000000000002</v>
+        <v>0.36341000000000001</v>
       </c>
       <c r="E12" s="2">
-        <v>0.63812999999999998</v>
+        <v>0.63853000000000004</v>
       </c>
       <c r="F12">
         <f>1-E12</f>
-        <v>0.36187000000000002</v>
+        <v>0.36146999999999996</v>
       </c>
       <c r="G12">
         <f>1-D12</f>
-        <v>0.61498999999999993</v>
+        <v>0.63658999999999999</v>
       </c>
       <c r="H12">
         <f>IF(E12&gt;G12,1,2)</f>
@@ -1588,7 +1609,7 @@
       </c>
       <c r="J12" s="1">
         <f>ABS(G12-E12)</f>
-        <v>2.3140000000000049E-2</v>
+        <v>1.9400000000000528E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1602,18 +1623,18 @@
         <v>2</v>
       </c>
       <c r="D13" s="2">
-        <v>0.21557000000000001</v>
+        <v>0.25881999999999999</v>
       </c>
       <c r="E13" s="2">
-        <v>0.59584000000000004</v>
+        <v>0.65939999999999999</v>
       </c>
       <c r="F13">
         <f>1-E13</f>
-        <v>0.40415999999999996</v>
+        <v>0.34060000000000001</v>
       </c>
       <c r="G13">
         <f>1-D13</f>
-        <v>0.78442999999999996</v>
+        <v>0.74117999999999995</v>
       </c>
       <c r="H13">
         <f>IF(E13&gt;G13,1,2)</f>
@@ -1625,7 +1646,7 @@
       </c>
       <c r="J13" s="1">
         <f>ABS(G13-E13)</f>
-        <v>0.18858999999999992</v>
+        <v>8.1779999999999964E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1639,18 +1660,18 @@
         <v>1</v>
       </c>
       <c r="D14" s="2">
-        <v>0.31207000000000001</v>
+        <v>0.27638000000000001</v>
       </c>
       <c r="E14" s="2">
-        <v>0.63151999999999997</v>
+        <v>0.67820999999999998</v>
       </c>
       <c r="F14">
         <f>1-E14</f>
-        <v>0.36848000000000003</v>
+        <v>0.32179000000000002</v>
       </c>
       <c r="G14">
         <f>1-D14</f>
-        <v>0.68792999999999993</v>
+        <v>0.72361999999999993</v>
       </c>
       <c r="H14">
         <f>IF(E14&gt;G14,1,2)</f>
@@ -1662,7 +1683,7 @@
       </c>
       <c r="J14" s="1">
         <f>ABS(G14-E14)</f>
-        <v>5.640999999999996E-2</v>
+        <v>4.540999999999995E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1676,18 +1697,18 @@
         <v>2</v>
       </c>
       <c r="D15" s="2">
-        <v>0.30617</v>
+        <v>0.26349</v>
       </c>
       <c r="E15" s="2">
-        <v>0.59536</v>
+        <v>0.63402999999999998</v>
       </c>
       <c r="F15">
         <f>1-E15</f>
-        <v>0.40464</v>
+        <v>0.36597000000000002</v>
       </c>
       <c r="G15">
         <f>1-D15</f>
-        <v>0.69382999999999995</v>
+        <v>0.73651</v>
       </c>
       <c r="H15">
         <f>IF(E15&gt;G15,1,2)</f>
@@ -1699,7 +1720,7 @@
       </c>
       <c r="J15" s="1">
         <f>ABS(G15-E15)</f>
-        <v>9.8469999999999946E-2</v>
+        <v>0.10248000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1713,30 +1734,30 @@
         <v>2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.34943999999999997</v>
+        <v>0.30096000000000001</v>
       </c>
       <c r="E16" s="2">
-        <v>0.68423</v>
+        <v>0.68516999999999995</v>
       </c>
       <c r="F16">
         <f>1-E16</f>
-        <v>0.31577</v>
+        <v>0.31483000000000005</v>
       </c>
       <c r="G16">
         <f>1-D16</f>
-        <v>0.65056000000000003</v>
+        <v>0.69903999999999999</v>
       </c>
       <c r="H16">
         <f>IF(E16&gt;G16,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16">
         <f>IF(H16=C16,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1">
         <f>ABS(G16-E16)</f>
-        <v>3.3669999999999978E-2</v>
+        <v>1.3870000000000049E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1750,18 +1771,18 @@
         <v>2</v>
       </c>
       <c r="D17" s="2">
-        <v>0.41648000000000002</v>
+        <v>0.36863000000000001</v>
       </c>
       <c r="E17" s="2">
-        <v>0.70540999999999998</v>
+        <v>0.67718</v>
       </c>
       <c r="F17">
         <f>1-E17</f>
-        <v>0.29459000000000002</v>
+        <v>0.32282</v>
       </c>
       <c r="G17">
         <f>1-D17</f>
-        <v>0.58352000000000004</v>
+        <v>0.63136999999999999</v>
       </c>
       <c r="H17">
         <f>IF(E17&gt;G17,1,2)</f>
@@ -1773,7 +1794,7 @@
       </c>
       <c r="J17" s="1">
         <f>ABS(G17-E17)</f>
-        <v>0.12188999999999994</v>
+        <v>4.5810000000000017E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1787,18 +1808,18 @@
         <v>2</v>
       </c>
       <c r="D18" s="2">
-        <v>0.29537999999999998</v>
+        <v>0.24063000000000001</v>
       </c>
       <c r="E18" s="2">
-        <v>0.68335000000000001</v>
+        <v>0.71804000000000001</v>
       </c>
       <c r="F18">
         <f>1-E18</f>
-        <v>0.31664999999999999</v>
+        <v>0.28195999999999999</v>
       </c>
       <c r="G18">
         <f>1-D18</f>
-        <v>0.70462000000000002</v>
+        <v>0.75936999999999999</v>
       </c>
       <c r="H18">
         <f>IF(E18&gt;G18,1,2)</f>
@@ -1810,7 +1831,7 @@
       </c>
       <c r="J18" s="1">
         <f>ABS(G18-E18)</f>
-        <v>2.1270000000000011E-2</v>
+        <v>4.1329999999999978E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1824,18 +1845,18 @@
         <v>2</v>
       </c>
       <c r="D19" s="2">
-        <v>0.28190999999999999</v>
+        <v>0.24901999999999999</v>
       </c>
       <c r="E19" s="2">
-        <v>0.67971000000000004</v>
+        <v>0.66615999999999997</v>
       </c>
       <c r="F19">
         <f>1-E19</f>
-        <v>0.32028999999999996</v>
+        <v>0.33384000000000003</v>
       </c>
       <c r="G19">
         <f>1-D19</f>
-        <v>0.71809000000000001</v>
+        <v>0.75097999999999998</v>
       </c>
       <c r="H19">
         <f>IF(E19&gt;G19,1,2)</f>
@@ -1847,7 +1868,7 @@
       </c>
       <c r="J19" s="1">
         <f>ABS(G19-E19)</f>
-        <v>3.837999999999997E-2</v>
+        <v>8.4820000000000007E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1861,30 +1882,30 @@
         <v>2</v>
       </c>
       <c r="D20" s="2">
-        <v>0.37724000000000002</v>
+        <v>0.33559</v>
       </c>
       <c r="E20" s="2">
-        <v>0.67652000000000001</v>
+        <v>0.66186999999999996</v>
       </c>
       <c r="F20">
         <f>1-E20</f>
-        <v>0.32347999999999999</v>
+        <v>0.33813000000000004</v>
       </c>
       <c r="G20">
         <f>1-D20</f>
-        <v>0.62275999999999998</v>
+        <v>0.66440999999999995</v>
       </c>
       <c r="H20">
         <f>IF(E20&gt;G20,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20">
         <f>IF(H20=C20,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1">
         <f>ABS(G20-E20)</f>
-        <v>5.376000000000003E-2</v>
+        <v>2.5399999999999867E-3</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1898,30 +1919,30 @@
         <v>2</v>
       </c>
       <c r="D21" s="2">
-        <v>0.35331000000000001</v>
+        <v>0.31489</v>
       </c>
       <c r="E21" s="2">
-        <v>0.67157999999999995</v>
+        <v>0.64937</v>
       </c>
       <c r="F21">
         <f>1-E21</f>
-        <v>0.32842000000000005</v>
+        <v>0.35063</v>
       </c>
       <c r="G21">
         <f>1-D21</f>
-        <v>0.64668999999999999</v>
+        <v>0.68511</v>
       </c>
       <c r="H21">
         <f>IF(E21&gt;G21,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21">
         <f>IF(H21=C21,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1">
         <f>ABS(G21-E21)</f>
-        <v>2.4889999999999968E-2</v>
+        <v>3.5739999999999994E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1935,18 +1956,18 @@
         <v>2</v>
       </c>
       <c r="D22" s="2">
-        <v>0.41541</v>
+        <v>0.36465999999999998</v>
       </c>
       <c r="E22" s="2">
-        <v>0.67972999999999995</v>
+        <v>0.63788999999999996</v>
       </c>
       <c r="F22">
         <f>1-E22</f>
-        <v>0.32027000000000005</v>
+        <v>0.36211000000000004</v>
       </c>
       <c r="G22">
         <f>1-D22</f>
-        <v>0.58458999999999994</v>
+        <v>0.63534000000000002</v>
       </c>
       <c r="H22">
         <f>IF(E22&gt;G22,1,2)</f>
@@ -1958,7 +1979,7 @@
       </c>
       <c r="J22" s="1">
         <f>ABS(G22-E22)</f>
-        <v>9.5140000000000002E-2</v>
+        <v>2.5499999999999412E-3</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1972,18 +1993,18 @@
         <v>2</v>
       </c>
       <c r="D23" s="2">
-        <v>0.26749000000000001</v>
+        <v>0.24410999999999999</v>
       </c>
       <c r="E23" s="2">
-        <v>0.68964000000000003</v>
+        <v>0.66856000000000004</v>
       </c>
       <c r="F23">
         <f>1-E23</f>
-        <v>0.31035999999999997</v>
+        <v>0.33143999999999996</v>
       </c>
       <c r="G23">
         <f>1-D23</f>
-        <v>0.73250999999999999</v>
+        <v>0.75588999999999995</v>
       </c>
       <c r="H23">
         <f>IF(E23&gt;G23,1,2)</f>
@@ -1995,7 +2016,7 @@
       </c>
       <c r="J23" s="1">
         <f>ABS(G23-E23)</f>
-        <v>4.2869999999999964E-2</v>
+        <v>8.7329999999999908E-2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2009,18 +2030,18 @@
         <v>2</v>
       </c>
       <c r="D24" s="2">
-        <v>0.28964000000000001</v>
+        <v>0.23691000000000001</v>
       </c>
       <c r="E24" s="2">
-        <v>0.6331</v>
+        <v>0.68303000000000003</v>
       </c>
       <c r="F24">
         <f>1-E24</f>
-        <v>0.3669</v>
+        <v>0.31696999999999997</v>
       </c>
       <c r="G24">
         <f>1-D24</f>
-        <v>0.71035999999999999</v>
+        <v>0.76309000000000005</v>
       </c>
       <c r="H24">
         <f>IF(E24&gt;G24,1,2)</f>
@@ -2032,7 +2053,7 @@
       </c>
       <c r="J24" s="1">
         <f>ABS(G24-E24)</f>
-        <v>7.7259999999999995E-2</v>
+        <v>8.006000000000002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2046,30 +2067,30 @@
         <v>1</v>
       </c>
       <c r="D25" s="2">
-        <v>0.35067999999999999</v>
+        <v>0.29249999999999998</v>
       </c>
       <c r="E25" s="2">
-        <v>0.69930000000000003</v>
+        <v>0.70408000000000004</v>
       </c>
       <c r="F25">
         <f>1-E25</f>
-        <v>0.30069999999999997</v>
+        <v>0.29591999999999996</v>
       </c>
       <c r="G25">
         <f>1-D25</f>
-        <v>0.64932000000000001</v>
+        <v>0.70750000000000002</v>
       </c>
       <c r="H25">
         <f>IF(E25&gt;G25,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25">
         <f>IF(H25=C25,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="1">
         <f>ABS(G25-E25)</f>
-        <v>4.9980000000000024E-2</v>
+        <v>3.4199999999999786E-3</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2083,30 +2104,30 @@
         <v>1</v>
       </c>
       <c r="D26" s="2">
-        <v>0.33732000000000001</v>
+        <v>0.28597</v>
       </c>
       <c r="E26" s="2">
-        <v>0.71074999999999999</v>
+        <v>0.69181999999999999</v>
       </c>
       <c r="F26">
         <f>1-E26</f>
-        <v>0.28925000000000001</v>
+        <v>0.30818000000000001</v>
       </c>
       <c r="G26">
         <f>1-D26</f>
-        <v>0.66267999999999994</v>
+        <v>0.71402999999999994</v>
       </c>
       <c r="H26">
         <f>IF(E26&gt;G26,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26">
         <f>IF(H26=C26,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="1">
         <f>ABS(G26-E26)</f>
-        <v>4.8070000000000057E-2</v>
+        <v>2.2209999999999952E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2120,30 +2141,30 @@
         <v>1</v>
       </c>
       <c r="D27" s="2">
-        <v>0.34240999999999999</v>
+        <v>0.31147999999999998</v>
       </c>
       <c r="E27" s="2">
-        <v>0.68862999999999996</v>
+        <v>0.65819000000000005</v>
       </c>
       <c r="F27">
         <f>1-E27</f>
-        <v>0.31137000000000004</v>
+        <v>0.34180999999999995</v>
       </c>
       <c r="G27">
         <f>1-D27</f>
-        <v>0.65759000000000001</v>
+        <v>0.68852000000000002</v>
       </c>
       <c r="H27">
         <f>IF(E27&gt;G27,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27">
         <f>IF(H27=C27,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="1">
         <f>ABS(G27-E27)</f>
-        <v>3.1039999999999957E-2</v>
+        <v>3.0329999999999968E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2157,18 +2178,18 @@
         <v>2</v>
       </c>
       <c r="D28" s="2">
-        <v>0.31376999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="E28" s="2">
-        <v>0.61165000000000003</v>
+        <v>0.60167000000000004</v>
       </c>
       <c r="F28">
         <f>1-E28</f>
-        <v>0.38834999999999997</v>
+        <v>0.39832999999999996</v>
       </c>
       <c r="G28">
         <f>1-D28</f>
-        <v>0.68623000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="H28">
         <f>IF(E28&gt;G28,1,2)</f>
@@ -2180,7 +2201,7 @@
       </c>
       <c r="J28" s="1">
         <f>ABS(G28-E28)</f>
-        <v>7.457999999999998E-2</v>
+        <v>9.8329999999999917E-2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2188,36 +2209,36 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" s="2">
-        <v>0.32307999999999998</v>
+        <v>0.34941</v>
       </c>
       <c r="E29" s="2">
-        <v>0.65276000000000001</v>
+        <v>0.69950000000000001</v>
       </c>
       <c r="F29">
         <f>1-E29</f>
-        <v>0.34723999999999999</v>
+        <v>0.30049999999999999</v>
       </c>
       <c r="G29">
         <f>1-D29</f>
-        <v>0.67691999999999997</v>
+        <v>0.65059</v>
       </c>
       <c r="H29">
         <f>IF(E29&gt;G29,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f>IF(H29=C29,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1">
         <f>ABS(G29-E29)</f>
-        <v>2.4159999999999959E-2</v>
+        <v>4.8910000000000009E-2</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -2225,28 +2246,28 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" s="2">
-        <v>0.38743</v>
+        <v>0.23252</v>
       </c>
       <c r="E30" s="2">
-        <v>0.69305000000000005</v>
+        <v>0.73995</v>
       </c>
       <c r="F30">
         <f>1-E30</f>
-        <v>0.30694999999999995</v>
+        <v>0.26005</v>
       </c>
       <c r="G30">
         <f>1-D30</f>
-        <v>0.61257000000000006</v>
+        <v>0.76747999999999994</v>
       </c>
       <c r="H30">
         <f>IF(E30&gt;G30,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30">
         <f>IF(H30=C30,1,0)</f>
@@ -2254,7 +2275,7 @@
       </c>
       <c r="J30" s="1">
         <f>ABS(G30-E30)</f>
-        <v>8.0479999999999996E-2</v>
+        <v>2.7529999999999943E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2262,28 +2283,28 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
-        <v>0.26956999999999998</v>
+        <v>0.28670000000000001</v>
       </c>
       <c r="E31" s="2">
-        <v>0.67247000000000001</v>
+        <v>0.71623999999999999</v>
       </c>
       <c r="F31">
         <f>1-E31</f>
-        <v>0.32752999999999999</v>
+        <v>0.28376000000000001</v>
       </c>
       <c r="G31">
         <f>1-D31</f>
-        <v>0.73043000000000002</v>
+        <v>0.71330000000000005</v>
       </c>
       <c r="H31">
         <f>IF(E31&gt;G31,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <f>IF(H31=C31,1,0)</f>
@@ -2291,7 +2312,7 @@
       </c>
       <c r="J31" s="1">
         <f>ABS(G31-E31)</f>
-        <v>5.7960000000000012E-2</v>
+        <v>2.9399999999999427E-3</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2305,18 +2326,18 @@
         <v>2</v>
       </c>
       <c r="D32" s="2">
-        <v>0.28062999999999999</v>
+        <v>0.24107000000000001</v>
       </c>
       <c r="E32" s="2">
-        <v>0.62444999999999995</v>
+        <v>0.66830000000000001</v>
       </c>
       <c r="F32">
         <f>1-E32</f>
-        <v>0.37555000000000005</v>
+        <v>0.33169999999999999</v>
       </c>
       <c r="G32">
         <f>1-D32</f>
-        <v>0.71937000000000006</v>
+        <v>0.75892999999999999</v>
       </c>
       <c r="H32">
         <f>IF(E32&gt;G32,1,2)</f>
@@ -2328,7 +2349,7 @@
       </c>
       <c r="J32" s="1">
         <f>ABS(G32-E32)</f>
-        <v>9.4920000000000115E-2</v>
+        <v>9.0629999999999988E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -2342,18 +2363,18 @@
         <v>1</v>
       </c>
       <c r="D33" s="2">
-        <v>0.32412000000000002</v>
+        <v>0.29069</v>
       </c>
       <c r="E33" s="2">
-        <v>0.65449000000000002</v>
+        <v>0.65125999999999995</v>
       </c>
       <c r="F33">
         <f>1-E33</f>
-        <v>0.34550999999999998</v>
+        <v>0.34874000000000005</v>
       </c>
       <c r="G33">
         <f>1-D33</f>
-        <v>0.67588000000000004</v>
+        <v>0.70931</v>
       </c>
       <c r="H33">
         <f>IF(E33&gt;G33,1,2)</f>
@@ -2365,7 +2386,7 @@
       </c>
       <c r="J33" s="1">
         <f>ABS(G33-E33)</f>
-        <v>2.139000000000002E-2</v>
+        <v>5.8050000000000046E-2</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -2379,18 +2400,18 @@
         <v>2</v>
       </c>
       <c r="D34" s="2">
-        <v>0.24990999999999999</v>
+        <v>0.23613999999999999</v>
       </c>
       <c r="E34" s="2">
-        <v>0.68432000000000004</v>
+        <v>0.69481999999999999</v>
       </c>
       <c r="F34">
         <f>1-E34</f>
-        <v>0.31567999999999996</v>
+        <v>0.30518000000000001</v>
       </c>
       <c r="G34">
         <f>1-D34</f>
-        <v>0.75009000000000003</v>
+        <v>0.76385999999999998</v>
       </c>
       <c r="H34">
         <f>IF(E34&gt;G34,1,2)</f>
@@ -2402,7 +2423,7 @@
       </c>
       <c r="J34" s="1">
         <f>ABS(G34-E34)</f>
-        <v>6.5769999999999995E-2</v>
+        <v>6.903999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -2416,18 +2437,18 @@
         <v>2</v>
       </c>
       <c r="D35" s="2">
-        <v>0.27251999999999998</v>
+        <v>0.22939999999999999</v>
       </c>
       <c r="E35" s="2">
-        <v>0.61780999999999997</v>
+        <v>0.70740999999999998</v>
       </c>
       <c r="F35">
         <f>1-E35</f>
-        <v>0.38219000000000003</v>
+        <v>0.29259000000000002</v>
       </c>
       <c r="G35">
         <f>1-D35</f>
-        <v>0.72748000000000002</v>
+        <v>0.77059999999999995</v>
       </c>
       <c r="H35">
         <f>IF(E35&gt;G35,1,2)</f>
@@ -2439,7 +2460,7 @@
       </c>
       <c r="J35" s="1">
         <f>ABS(G35-E35)</f>
-        <v>0.10967000000000005</v>
+        <v>6.3189999999999968E-2</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -2453,18 +2474,18 @@
         <v>1</v>
       </c>
       <c r="D36" s="2">
-        <v>0.38083</v>
+        <v>0.37480999999999998</v>
       </c>
       <c r="E36" s="2">
-        <v>0.66847000000000001</v>
+        <v>0.70474000000000003</v>
       </c>
       <c r="F36">
         <f>1-E36</f>
-        <v>0.33152999999999999</v>
+        <v>0.29525999999999997</v>
       </c>
       <c r="G36">
         <f>1-D36</f>
-        <v>0.61917</v>
+        <v>0.62519000000000002</v>
       </c>
       <c r="H36">
         <f>IF(E36&gt;G36,1,2)</f>
@@ -2476,7 +2497,7 @@
       </c>
       <c r="J36" s="1">
         <f>ABS(G36-E36)</f>
-        <v>4.930000000000001E-2</v>
+        <v>7.955000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -2490,18 +2511,18 @@
         <v>2</v>
       </c>
       <c r="D37" s="2">
-        <v>0.27840999999999999</v>
+        <v>0.23610999999999999</v>
       </c>
       <c r="E37" s="2">
-        <v>0.64629999999999999</v>
+        <v>0.66461999999999999</v>
       </c>
       <c r="F37">
         <f>1-E37</f>
-        <v>0.35370000000000001</v>
+        <v>0.33538000000000001</v>
       </c>
       <c r="G37">
         <f>1-D37</f>
-        <v>0.72158999999999995</v>
+        <v>0.76388999999999996</v>
       </c>
       <c r="H37">
         <f>IF(E37&gt;G37,1,2)</f>
@@ -2513,7 +2534,7 @@
       </c>
       <c r="J37" s="1">
         <f>ABS(G37-E37)</f>
-        <v>7.5289999999999968E-2</v>
+        <v>9.9269999999999969E-2</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2527,18 +2548,18 @@
         <v>1</v>
       </c>
       <c r="D38" s="2">
-        <v>0.47688999999999998</v>
+        <v>0.31523000000000001</v>
       </c>
       <c r="E38" s="2">
-        <v>0.75400999999999996</v>
+        <v>0.71828000000000003</v>
       </c>
       <c r="F38">
         <f>1-E38</f>
-        <v>0.24599000000000004</v>
+        <v>0.28171999999999997</v>
       </c>
       <c r="G38">
         <f>1-D38</f>
-        <v>0.52310999999999996</v>
+        <v>0.68476999999999999</v>
       </c>
       <c r="H38">
         <f>IF(E38&gt;G38,1,2)</f>
@@ -2550,7 +2571,7 @@
       </c>
       <c r="J38" s="1">
         <f>ABS(G38-E38)</f>
-        <v>0.23089999999999999</v>
+        <v>3.351000000000004E-2</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -2564,30 +2585,30 @@
         <v>1</v>
       </c>
       <c r="D39" s="2">
-        <v>0.38052000000000002</v>
+        <v>0.17444000000000001</v>
       </c>
       <c r="E39" s="2">
-        <v>0.75741000000000003</v>
+        <v>0.76361999999999997</v>
       </c>
       <c r="F39">
         <f>1-E39</f>
-        <v>0.24258999999999997</v>
+        <v>0.23638000000000003</v>
       </c>
       <c r="G39">
         <f>1-D39</f>
-        <v>0.61948000000000003</v>
+        <v>0.82555999999999996</v>
       </c>
       <c r="H39">
         <f>IF(E39&gt;G39,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39">
         <f>IF(H39=C39,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="1">
         <f>ABS(G39-E39)</f>
-        <v>0.13793</v>
+        <v>6.1939999999999995E-2</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -2601,30 +2622,30 @@
         <v>1</v>
       </c>
       <c r="D40" s="2">
-        <v>0.39036999999999999</v>
+        <v>0.14077000000000001</v>
       </c>
       <c r="E40" s="2">
-        <v>0.73663000000000001</v>
+        <v>0.73868</v>
       </c>
       <c r="F40">
         <f>1-E40</f>
-        <v>0.26336999999999999</v>
+        <v>0.26132</v>
       </c>
       <c r="G40">
         <f>1-D40</f>
-        <v>0.60963000000000001</v>
+        <v>0.85922999999999994</v>
       </c>
       <c r="H40">
         <f>IF(E40&gt;G40,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I40">
         <f>IF(H40=C40,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="1">
         <f>ABS(G40-E40)</f>
-        <v>0.127</v>
+        <v>0.12054999999999993</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2638,30 +2659,30 @@
         <v>1</v>
       </c>
       <c r="D41" s="2">
-        <v>0.42210999999999999</v>
+        <v>0.25196000000000002</v>
       </c>
       <c r="E41" s="2">
-        <v>0.67259999999999998</v>
+        <v>0.72509999999999997</v>
       </c>
       <c r="F41">
         <f>1-E41</f>
-        <v>0.32740000000000002</v>
+        <v>0.27490000000000003</v>
       </c>
       <c r="G41">
         <f>1-D41</f>
-        <v>0.57789000000000001</v>
+        <v>0.74804000000000004</v>
       </c>
       <c r="H41">
         <f>IF(E41&gt;G41,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41">
         <f>IF(H41=C41,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="1">
         <f>ABS(G41-E41)</f>
-        <v>9.4709999999999961E-2</v>
+        <v>2.2940000000000071E-2</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -2675,30 +2696,30 @@
         <v>2</v>
       </c>
       <c r="D42" s="2">
-        <v>0.39711000000000002</v>
+        <v>0.18506</v>
       </c>
       <c r="E42" s="2">
-        <v>0.77800999999999998</v>
+        <v>0.77825999999999995</v>
       </c>
       <c r="F42">
         <f>1-E42</f>
-        <v>0.22199000000000002</v>
+        <v>0.22174000000000005</v>
       </c>
       <c r="G42">
         <f>1-D42</f>
-        <v>0.60288999999999993</v>
+        <v>0.81494</v>
       </c>
       <c r="H42">
         <f>IF(E42&gt;G42,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42">
         <f>IF(H42=C42,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="1">
         <f>ABS(G42-E42)</f>
-        <v>0.17512000000000005</v>
+        <v>3.6680000000000046E-2</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -2712,30 +2733,30 @@
         <v>1</v>
       </c>
       <c r="D43" s="2">
-        <v>0.42232999999999998</v>
+        <v>0.24687000000000001</v>
       </c>
       <c r="E43" s="2">
-        <v>0.76454999999999995</v>
+        <v>0.74299000000000004</v>
       </c>
       <c r="F43">
         <f>1-E43</f>
-        <v>0.23545000000000005</v>
+        <v>0.25700999999999996</v>
       </c>
       <c r="G43">
         <f>1-D43</f>
-        <v>0.57767000000000002</v>
+        <v>0.75312999999999997</v>
       </c>
       <c r="H43">
         <f>IF(E43&gt;G43,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43">
         <f>IF(H43=C43,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" s="1">
         <f>ABS(G43-E43)</f>
-        <v>0.18687999999999994</v>
+        <v>1.0139999999999927E-2</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -2749,18 +2770,18 @@
         <v>2</v>
       </c>
       <c r="D44" s="2">
-        <v>0.29710999999999999</v>
+        <v>0.23069999999999999</v>
       </c>
       <c r="E44" s="2">
-        <v>0.7258</v>
+        <v>0.80686999999999998</v>
       </c>
       <c r="F44">
         <f>1-E44</f>
-        <v>0.2742</v>
+        <v>0.19313000000000002</v>
       </c>
       <c r="G44">
         <f>1-D44</f>
-        <v>0.70289000000000001</v>
+        <v>0.76929999999999998</v>
       </c>
       <c r="H44">
         <f>IF(E44&gt;G44,1,2)</f>
@@ -2772,7 +2793,7 @@
       </c>
       <c r="J44" s="1">
         <f>ABS(G44-E44)</f>
-        <v>2.2909999999999986E-2</v>
+        <v>3.7569999999999992E-2</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -2786,18 +2807,18 @@
         <v>1</v>
       </c>
       <c r="D45" s="2">
-        <v>0.32579000000000002</v>
+        <v>0.23455000000000001</v>
       </c>
       <c r="E45" s="2">
-        <v>0.74172000000000005</v>
+        <v>0.79869999999999997</v>
       </c>
       <c r="F45">
         <f>1-E45</f>
-        <v>0.25827999999999995</v>
+        <v>0.20130000000000003</v>
       </c>
       <c r="G45">
         <f>1-D45</f>
-        <v>0.67420999999999998</v>
+        <v>0.76544999999999996</v>
       </c>
       <c r="H45">
         <f>IF(E45&gt;G45,1,2)</f>
@@ -2809,7 +2830,7 @@
       </c>
       <c r="J45" s="1">
         <f>ABS(G45-E45)</f>
-        <v>6.751000000000007E-2</v>
+        <v>3.3250000000000002E-2</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2823,30 +2844,30 @@
         <v>2</v>
       </c>
       <c r="D46" s="2">
-        <v>0.31942999999999999</v>
+        <v>0.22170999999999999</v>
       </c>
       <c r="E46" s="2">
-        <v>0.70526999999999995</v>
+        <v>0.76483000000000001</v>
       </c>
       <c r="F46">
         <f>1-E46</f>
-        <v>0.29473000000000005</v>
+        <v>0.23516999999999999</v>
       </c>
       <c r="G46">
         <f>1-D46</f>
-        <v>0.68057000000000001</v>
+        <v>0.77829000000000004</v>
       </c>
       <c r="H46">
         <f>IF(E46&gt;G46,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46">
         <f>IF(H46=C46,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="1">
         <f>ABS(G46-E46)</f>
-        <v>2.4699999999999944E-2</v>
+        <v>1.3460000000000027E-2</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2860,18 +2881,18 @@
         <v>1</v>
       </c>
       <c r="D47" s="2">
-        <v>0.36302000000000001</v>
+        <v>0.32146000000000002</v>
       </c>
       <c r="E47" s="2">
-        <v>0.71304999999999996</v>
+        <v>0.78446000000000005</v>
       </c>
       <c r="F47">
         <f>1-E47</f>
-        <v>0.28695000000000004</v>
+        <v>0.21553999999999995</v>
       </c>
       <c r="G47">
         <f>1-D47</f>
-        <v>0.63697999999999999</v>
+        <v>0.67853999999999992</v>
       </c>
       <c r="H47">
         <f>IF(E47&gt;G47,1,2)</f>
@@ -2883,7 +2904,7 @@
       </c>
       <c r="J47" s="1">
         <f>ABS(G47-E47)</f>
-        <v>7.6069999999999971E-2</v>
+        <v>0.10592000000000013</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -2897,18 +2918,18 @@
         <v>1</v>
       </c>
       <c r="D48" s="2">
-        <v>0.19367999999999999</v>
+        <v>0.25269999999999998</v>
       </c>
       <c r="E48" s="2">
-        <v>0.75882000000000005</v>
+        <v>0.71992</v>
       </c>
       <c r="F48">
         <f>1-E48</f>
-        <v>0.24117999999999995</v>
+        <v>0.28008</v>
       </c>
       <c r="G48">
         <f>1-D48</f>
-        <v>0.80632000000000004</v>
+        <v>0.74730000000000008</v>
       </c>
       <c r="H48">
         <f>IF(E48&gt;G48,1,2)</f>
@@ -2920,7 +2941,7 @@
       </c>
       <c r="J48" s="1">
         <f>ABS(G48-E48)</f>
-        <v>4.7499999999999987E-2</v>
+        <v>2.7380000000000071E-2</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -2934,18 +2955,18 @@
         <v>2</v>
       </c>
       <c r="D49" s="2">
-        <v>0.41133999999999998</v>
+        <v>0.42337000000000002</v>
       </c>
       <c r="E49" s="2">
-        <v>0.67278000000000004</v>
+        <v>0.6663</v>
       </c>
       <c r="F49">
         <f>1-E49</f>
-        <v>0.32721999999999996</v>
+        <v>0.3337</v>
       </c>
       <c r="G49">
         <f>1-D49</f>
-        <v>0.58865999999999996</v>
+        <v>0.57662999999999998</v>
       </c>
       <c r="H49">
         <f>IF(E49&gt;G49,1,2)</f>
@@ -2957,7 +2978,7 @@
       </c>
       <c r="J49" s="1">
         <f>ABS(G49-E49)</f>
-        <v>8.4120000000000084E-2</v>
+        <v>8.9670000000000027E-2</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -2971,18 +2992,18 @@
         <v>1</v>
       </c>
       <c r="D50" s="2">
-        <v>0.38162000000000001</v>
+        <v>0.41757</v>
       </c>
       <c r="E50" s="2">
-        <v>0.65846000000000005</v>
+        <v>0.66585000000000005</v>
       </c>
       <c r="F50">
         <f>1-E50</f>
-        <v>0.34153999999999995</v>
+        <v>0.33414999999999995</v>
       </c>
       <c r="G50">
         <f>1-D50</f>
-        <v>0.61837999999999993</v>
+        <v>0.58243</v>
       </c>
       <c r="H50">
         <f>IF(E50&gt;G50,1,2)</f>
@@ -2994,7 +3015,7 @@
       </c>
       <c r="J50" s="1">
         <f>ABS(G50-E50)</f>
-        <v>4.0080000000000116E-2</v>
+        <v>8.342000000000005E-2</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -3008,30 +3029,30 @@
         <v>1</v>
       </c>
       <c r="D51" s="2">
-        <v>0.34587000000000001</v>
+        <v>0.35797000000000001</v>
       </c>
       <c r="E51" s="2">
-        <v>0.63041000000000003</v>
+        <v>0.6583</v>
       </c>
       <c r="F51">
         <f>1-E51</f>
-        <v>0.36958999999999997</v>
+        <v>0.3417</v>
       </c>
       <c r="G51">
         <f>1-D51</f>
-        <v>0.65412999999999999</v>
+        <v>0.64202999999999999</v>
       </c>
       <c r="H51">
         <f>IF(E51&gt;G51,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I51">
         <f>IF(H51=C51,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" s="1">
         <f>ABS(G51-E51)</f>
-        <v>2.3719999999999963E-2</v>
+        <v>1.6270000000000007E-2</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3045,18 +3066,18 @@
         <v>1</v>
       </c>
       <c r="D52" s="2">
-        <v>0.38245000000000001</v>
+        <v>0.40699000000000002</v>
       </c>
       <c r="E52" s="2">
-        <v>0.66522000000000003</v>
+        <v>0.64548000000000005</v>
       </c>
       <c r="F52">
         <f>1-E52</f>
-        <v>0.33477999999999997</v>
+        <v>0.35451999999999995</v>
       </c>
       <c r="G52">
         <f>1-D52</f>
-        <v>0.61755000000000004</v>
+        <v>0.59301000000000004</v>
       </c>
       <c r="H52">
         <f>IF(E52&gt;G52,1,2)</f>
@@ -3068,7 +3089,7 @@
       </c>
       <c r="J52" s="1">
         <f>ABS(G52-E52)</f>
-        <v>4.766999999999999E-2</v>
+        <v>5.2470000000000017E-2</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3082,30 +3103,30 @@
         <v>1</v>
       </c>
       <c r="D53" s="2">
-        <v>0.32638</v>
+        <v>0.33976000000000001</v>
       </c>
       <c r="E53" s="2">
-        <v>0.62836999999999998</v>
+        <v>0.68881999999999999</v>
       </c>
       <c r="F53">
         <f>1-E53</f>
-        <v>0.37163000000000002</v>
+        <v>0.31118000000000001</v>
       </c>
       <c r="G53">
         <f>1-D53</f>
-        <v>0.67362</v>
+        <v>0.66023999999999994</v>
       </c>
       <c r="H53">
         <f>IF(E53&gt;G53,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53">
         <f>IF(H53=C53,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" s="1">
         <f>ABS(G53-E53)</f>
-        <v>4.5250000000000012E-2</v>
+        <v>2.858000000000005E-2</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -3119,18 +3140,18 @@
         <v>2</v>
       </c>
       <c r="D54" s="2">
-        <v>0.44308999999999998</v>
+        <v>0.48466999999999999</v>
       </c>
       <c r="E54" s="2">
-        <v>0.68145999999999995</v>
+        <v>0.69245000000000001</v>
       </c>
       <c r="F54">
         <f>1-E54</f>
-        <v>0.31854000000000005</v>
+        <v>0.30754999999999999</v>
       </c>
       <c r="G54">
         <f>1-D54</f>
-        <v>0.55691000000000002</v>
+        <v>0.51533000000000007</v>
       </c>
       <c r="H54">
         <f>IF(E54&gt;G54,1,2)</f>
@@ -3142,7 +3163,7 @@
       </c>
       <c r="J54" s="1">
         <f>ABS(G54-E54)</f>
-        <v>0.12454999999999994</v>
+        <v>0.17711999999999994</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -3156,18 +3177,18 @@
         <v>1</v>
       </c>
       <c r="D55" s="2">
-        <v>0.44681999999999999</v>
+        <v>0.46303</v>
       </c>
       <c r="E55" s="2">
-        <v>0.67218999999999995</v>
+        <v>0.65539000000000003</v>
       </c>
       <c r="F55">
         <f>1-E55</f>
-        <v>0.32781000000000005</v>
+        <v>0.34460999999999997</v>
       </c>
       <c r="G55">
         <f>1-D55</f>
-        <v>0.55318000000000001</v>
+        <v>0.53696999999999995</v>
       </c>
       <c r="H55">
         <f>IF(E55&gt;G55,1,2)</f>
@@ -3179,7 +3200,7 @@
       </c>
       <c r="J55" s="1">
         <f>ABS(G55-E55)</f>
-        <v>0.11900999999999995</v>
+        <v>0.11842000000000008</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -3193,18 +3214,18 @@
         <v>1</v>
       </c>
       <c r="D56" s="2">
-        <v>0.34758</v>
+        <v>0.33504</v>
       </c>
       <c r="E56" s="2">
-        <v>0.64890000000000003</v>
+        <v>0.65188999999999997</v>
       </c>
       <c r="F56">
         <f>1-E56</f>
-        <v>0.35109999999999997</v>
+        <v>0.34811000000000003</v>
       </c>
       <c r="G56">
         <f>1-D56</f>
-        <v>0.65242</v>
+        <v>0.66496</v>
       </c>
       <c r="H56">
         <f>IF(E56&gt;G56,1,2)</f>
@@ -3216,7 +3237,7 @@
       </c>
       <c r="J56" s="1">
         <f>ABS(G56-E56)</f>
-        <v>3.5199999999999676E-3</v>
+        <v>1.3070000000000026E-2</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -3230,18 +3251,18 @@
         <v>2</v>
       </c>
       <c r="D57" s="2">
-        <v>0.24868999999999999</v>
+        <v>0.24984000000000001</v>
       </c>
       <c r="E57" s="2">
-        <v>0.60412999999999994</v>
+        <v>0.67884999999999995</v>
       </c>
       <c r="F57">
         <f>1-E57</f>
-        <v>0.39587000000000006</v>
+        <v>0.32115000000000005</v>
       </c>
       <c r="G57">
         <f>1-D57</f>
-        <v>0.75131000000000003</v>
+        <v>0.75015999999999994</v>
       </c>
       <c r="H57">
         <f>IF(E57&gt;G57,1,2)</f>
@@ -3253,7 +3274,7 @@
       </c>
       <c r="J57" s="1">
         <f>ABS(G57-E57)</f>
-        <v>0.14718000000000009</v>
+        <v>7.1309999999999985E-2</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -3267,18 +3288,18 @@
         <v>2</v>
       </c>
       <c r="D58" s="2">
-        <v>0.30820999999999998</v>
+        <v>0.30823</v>
       </c>
       <c r="E58" s="2">
-        <v>0.59213000000000005</v>
+        <v>0.58892</v>
       </c>
       <c r="F58">
         <f>1-E58</f>
-        <v>0.40786999999999995</v>
+        <v>0.41108</v>
       </c>
       <c r="G58">
         <f>1-D58</f>
-        <v>0.69179000000000002</v>
+        <v>0.69177</v>
       </c>
       <c r="H58">
         <f>IF(E58&gt;G58,1,2)</f>
@@ -3290,7 +3311,7 @@
       </c>
       <c r="J58" s="1">
         <f>ABS(G58-E58)</f>
-        <v>9.9659999999999971E-2</v>
+        <v>0.10285</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -3304,18 +3325,18 @@
         <v>2</v>
       </c>
       <c r="D59" s="2">
-        <v>0.22403999999999999</v>
+        <v>0.24578</v>
       </c>
       <c r="E59" s="2">
-        <v>0.62475999999999998</v>
+        <v>0.63163000000000002</v>
       </c>
       <c r="F59">
         <f>1-E59</f>
-        <v>0.37524000000000002</v>
+        <v>0.36836999999999998</v>
       </c>
       <c r="G59">
         <f>1-D59</f>
-        <v>0.77595999999999998</v>
+        <v>0.75422</v>
       </c>
       <c r="H59">
         <f>IF(E59&gt;G59,1,2)</f>
@@ -3327,7 +3348,7 @@
       </c>
       <c r="J59" s="1">
         <f>ABS(G59-E59)</f>
-        <v>0.1512</v>
+        <v>0.12258999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -3341,18 +3362,18 @@
         <v>2</v>
       </c>
       <c r="D60" s="2">
-        <v>0.36253999999999997</v>
+        <v>0.35893999999999998</v>
       </c>
       <c r="E60" s="2">
-        <v>0.61282999999999999</v>
+        <v>0.60168999999999995</v>
       </c>
       <c r="F60">
         <f>1-E60</f>
-        <v>0.38717000000000001</v>
+        <v>0.39831000000000005</v>
       </c>
       <c r="G60">
         <f>1-D60</f>
-        <v>0.63746000000000003</v>
+        <v>0.64105999999999996</v>
       </c>
       <c r="H60">
         <f>IF(E60&gt;G60,1,2)</f>
@@ -3364,7 +3385,7 @@
       </c>
       <c r="J60" s="1">
         <f>ABS(G60-E60)</f>
-        <v>2.4630000000000041E-2</v>
+        <v>3.9370000000000016E-2</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -3378,18 +3399,18 @@
         <v>1</v>
       </c>
       <c r="D61" s="2">
-        <v>0.32528000000000001</v>
+        <v>0.32456000000000002</v>
       </c>
       <c r="E61" s="2">
-        <v>0.61921000000000004</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="F61">
         <f>1-E61</f>
-        <v>0.38078999999999996</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="G61">
         <f>1-D61</f>
-        <v>0.67471999999999999</v>
+        <v>0.67544000000000004</v>
       </c>
       <c r="H61">
         <f>IF(E61&gt;G61,1,2)</f>
@@ -3401,7 +3422,7 @@
       </c>
       <c r="J61" s="1">
         <f>ABS(G61-E61)</f>
-        <v>5.5509999999999948E-2</v>
+        <v>3.9440000000000031E-2</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -3415,30 +3436,30 @@
         <v>2</v>
       </c>
       <c r="D62" s="2">
-        <v>0.36760999999999999</v>
+        <v>0.39215</v>
       </c>
       <c r="E62" s="2">
-        <v>0.60038000000000002</v>
+        <v>0.64426000000000005</v>
       </c>
       <c r="F62">
         <f>1-E62</f>
-        <v>0.39961999999999998</v>
+        <v>0.35573999999999995</v>
       </c>
       <c r="G62">
         <f>1-D62</f>
-        <v>0.63239000000000001</v>
+        <v>0.60785</v>
       </c>
       <c r="H62">
         <f>IF(E62&gt;G62,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62">
         <f>IF(H62=C62,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="1">
         <f>ABS(G62-E62)</f>
-        <v>3.2009999999999983E-2</v>
+        <v>3.6410000000000053E-2</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -3452,18 +3473,18 @@
         <v>2</v>
       </c>
       <c r="D63" s="2">
-        <v>0.3785</v>
+        <v>0.36381999999999998</v>
       </c>
       <c r="E63" s="2">
-        <v>0.58818999999999999</v>
+        <v>0.60980999999999996</v>
       </c>
       <c r="F63">
         <f>1-E63</f>
-        <v>0.41181000000000001</v>
+        <v>0.39019000000000004</v>
       </c>
       <c r="G63">
         <f>1-D63</f>
-        <v>0.62149999999999994</v>
+        <v>0.63617999999999997</v>
       </c>
       <c r="H63">
         <f>IF(E63&gt;G63,1,2)</f>
@@ -3475,7 +3496,7 @@
       </c>
       <c r="J63" s="1">
         <f>ABS(G63-E63)</f>
-        <v>3.3309999999999951E-2</v>
+        <v>2.6370000000000005E-2</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -3489,18 +3510,18 @@
         <v>1</v>
       </c>
       <c r="D64" s="2">
-        <v>0.29164000000000001</v>
+        <v>0.29322999999999999</v>
       </c>
       <c r="E64" s="2">
-        <v>0.63661999999999996</v>
+        <v>0.65508999999999995</v>
       </c>
       <c r="F64">
         <f>1-E64</f>
-        <v>0.36338000000000004</v>
+        <v>0.34491000000000005</v>
       </c>
       <c r="G64">
         <f>1-D64</f>
-        <v>0.70835999999999999</v>
+        <v>0.70677000000000001</v>
       </c>
       <c r="H64">
         <f>IF(E64&gt;G64,1,2)</f>
@@ -3512,7 +3533,7 @@
       </c>
       <c r="J64" s="1">
         <f>ABS(G64-E64)</f>
-        <v>7.1740000000000026E-2</v>
+        <v>5.1680000000000059E-2</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -3526,18 +3547,18 @@
         <v>1</v>
       </c>
       <c r="D65" s="2">
-        <v>0.29699999999999999</v>
+        <v>0.31402000000000002</v>
       </c>
       <c r="E65" s="2">
-        <v>0.61880000000000002</v>
+        <v>0.62456999999999996</v>
       </c>
       <c r="F65">
         <f>1-E65</f>
-        <v>0.38119999999999998</v>
+        <v>0.37543000000000004</v>
       </c>
       <c r="G65">
         <f>1-D65</f>
-        <v>0.70300000000000007</v>
+        <v>0.68598000000000003</v>
       </c>
       <c r="H65">
         <f>IF(E65&gt;G65,1,2)</f>
@@ -3549,7 +3570,7 @@
       </c>
       <c r="J65" s="1">
         <f>ABS(G65-E65)</f>
-        <v>8.4200000000000053E-2</v>
+        <v>6.1410000000000076E-2</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -3563,30 +3584,30 @@
         <v>1</v>
       </c>
       <c r="D66" s="2">
-        <v>0.29587999999999998</v>
+        <v>0.27089999999999997</v>
       </c>
       <c r="E66" s="2">
-        <v>0.69125000000000003</v>
+        <v>0.74521999999999999</v>
       </c>
       <c r="F66">
         <f>1-E66</f>
-        <v>0.30874999999999997</v>
+        <v>0.25478000000000001</v>
       </c>
       <c r="G66">
         <f>1-D66</f>
-        <v>0.70412000000000008</v>
+        <v>0.72910000000000008</v>
       </c>
       <c r="H66">
         <f>IF(E66&gt;G66,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I66">
         <f>IF(H66=C66,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66" s="1">
         <f>ABS(G66-E66)</f>
-        <v>1.2870000000000048E-2</v>
+        <v>1.6119999999999912E-2</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -3600,18 +3621,18 @@
         <v>2</v>
       </c>
       <c r="D67" s="2">
-        <v>0.35466999999999999</v>
+        <v>0.30342999999999998</v>
       </c>
       <c r="E67" s="2">
-        <v>0.61326999999999998</v>
+        <v>0.63478000000000001</v>
       </c>
       <c r="F67">
         <f>1-E67</f>
-        <v>0.38673000000000002</v>
+        <v>0.36521999999999999</v>
       </c>
       <c r="G67">
         <f>1-D67</f>
-        <v>0.64532999999999996</v>
+        <v>0.69657000000000002</v>
       </c>
       <c r="H67">
         <f>IF(E67&gt;G67,1,2)</f>
@@ -3623,7 +3644,7 @@
       </c>
       <c r="J67" s="1">
         <f>ABS(G67-E67)</f>
-        <v>3.2059999999999977E-2</v>
+        <v>6.1790000000000012E-2</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -3637,18 +3658,18 @@
         <v>1</v>
       </c>
       <c r="D68" s="2">
-        <v>0.36618000000000001</v>
+        <v>0.36621999999999999</v>
       </c>
       <c r="E68" s="2">
-        <v>0.67334000000000005</v>
+        <v>0.70938000000000001</v>
       </c>
       <c r="F68">
         <f>1-E68</f>
-        <v>0.32665999999999995</v>
+        <v>0.29061999999999999</v>
       </c>
       <c r="G68">
         <f>1-D68</f>
-        <v>0.63382000000000005</v>
+        <v>0.63378000000000001</v>
       </c>
       <c r="H68">
         <f>IF(E68&gt;G68,1,2)</f>
@@ -3660,7 +3681,7 @@
       </c>
       <c r="J68" s="1">
         <f>ABS(G68-E68)</f>
-        <v>3.952E-2</v>
+        <v>7.5600000000000001E-2</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -3674,18 +3695,18 @@
         <v>1</v>
       </c>
       <c r="D69" s="2">
-        <v>0.37961</v>
+        <v>0.30176999999999998</v>
       </c>
       <c r="E69" s="2">
-        <v>0.66379999999999995</v>
+        <v>0.70689000000000002</v>
       </c>
       <c r="F69">
         <f>1-E69</f>
-        <v>0.33620000000000005</v>
+        <v>0.29310999999999998</v>
       </c>
       <c r="G69">
         <f>1-D69</f>
-        <v>0.62039</v>
+        <v>0.69823000000000002</v>
       </c>
       <c r="H69">
         <f>IF(E69&gt;G69,1,2)</f>
@@ -3697,7 +3718,7 @@
       </c>
       <c r="J69" s="1">
         <f>ABS(G69-E69)</f>
-        <v>4.3409999999999949E-2</v>
+        <v>8.660000000000001E-3</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -3711,18 +3732,18 @@
         <v>2</v>
       </c>
       <c r="D70" s="2">
-        <v>0.19980999999999999</v>
+        <v>9.9260000000000001E-2</v>
       </c>
       <c r="E70" s="2">
-        <v>0.73801000000000005</v>
+        <v>0.76870000000000005</v>
       </c>
       <c r="F70">
         <f>1-E70</f>
-        <v>0.26198999999999995</v>
+        <v>0.23129999999999995</v>
       </c>
       <c r="G70">
         <f>1-D70</f>
-        <v>0.80018999999999996</v>
+        <v>0.90073999999999999</v>
       </c>
       <c r="H70">
         <f>IF(E70&gt;G70,1,2)</f>
@@ -3734,7 +3755,7 @@
       </c>
       <c r="J70" s="1">
         <f>ABS(G70-E70)</f>
-        <v>6.2179999999999902E-2</v>
+        <v>0.13203999999999994</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -3748,30 +3769,30 @@
         <v>2</v>
       </c>
       <c r="D71" s="2">
-        <v>0.36258000000000001</v>
+        <v>0.29892999999999997</v>
       </c>
       <c r="E71" s="2">
-        <v>0.64502000000000004</v>
+        <v>0.67869999999999997</v>
       </c>
       <c r="F71">
         <f>1-E71</f>
-        <v>0.35497999999999996</v>
+        <v>0.32130000000000003</v>
       </c>
       <c r="G71">
         <f>1-D71</f>
-        <v>0.63741999999999999</v>
+        <v>0.70107000000000008</v>
       </c>
       <c r="H71">
         <f>IF(E71&gt;G71,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I71">
         <f>IF(H71=C71,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" s="1">
         <f>ABS(G71-E71)</f>
-        <v>7.6000000000000512E-3</v>
+        <v>2.2370000000000112E-2</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -3785,18 +3806,18 @@
         <v>2</v>
       </c>
       <c r="D72" s="2">
-        <v>0.35665999999999998</v>
+        <v>0.29094999999999999</v>
       </c>
       <c r="E72" s="2">
-        <v>0.56945000000000001</v>
+        <v>0.68156000000000005</v>
       </c>
       <c r="F72">
         <f>1-E72</f>
-        <v>0.43054999999999999</v>
+        <v>0.31843999999999995</v>
       </c>
       <c r="G72">
         <f>1-D72</f>
-        <v>0.64334000000000002</v>
+        <v>0.70904999999999996</v>
       </c>
       <c r="H72">
         <f>IF(E72&gt;G72,1,2)</f>
@@ -3808,7 +3829,7 @@
       </c>
       <c r="J72" s="1">
         <f>ABS(G72-E72)</f>
-        <v>7.3890000000000011E-2</v>
+        <v>2.7489999999999903E-2</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -3822,18 +3843,18 @@
         <v>2</v>
       </c>
       <c r="D73" s="2">
-        <v>0.21909999999999999</v>
+        <v>0.19459000000000001</v>
       </c>
       <c r="E73" s="2">
-        <v>0.66593999999999998</v>
+        <v>0.66037000000000001</v>
       </c>
       <c r="F73">
         <f>1-E73</f>
-        <v>0.33406000000000002</v>
+        <v>0.33962999999999999</v>
       </c>
       <c r="G73">
         <f>1-D73</f>
-        <v>0.78090000000000004</v>
+        <v>0.80540999999999996</v>
       </c>
       <c r="H73">
         <f>IF(E73&gt;G73,1,2)</f>
@@ -3845,7 +3866,7 @@
       </c>
       <c r="J73" s="1">
         <f>ABS(G73-E73)</f>
-        <v>0.11496000000000006</v>
+        <v>0.14503999999999995</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -3859,18 +3880,18 @@
         <v>1</v>
       </c>
       <c r="D74" s="2">
-        <v>0.33276</v>
+        <v>0.28328999999999999</v>
       </c>
       <c r="E74" s="2">
-        <v>0.58418000000000003</v>
+        <v>0.68320999999999998</v>
       </c>
       <c r="F74">
         <f>1-E74</f>
-        <v>0.41581999999999997</v>
+        <v>0.31679000000000002</v>
       </c>
       <c r="G74">
         <f>1-D74</f>
-        <v>0.66724000000000006</v>
+        <v>0.71670999999999996</v>
       </c>
       <c r="H74">
         <f>IF(E74&gt;G74,1,2)</f>
@@ -3882,7 +3903,7 @@
       </c>
       <c r="J74" s="1">
         <f>ABS(G74-E74)</f>
-        <v>8.3060000000000023E-2</v>
+        <v>3.3499999999999974E-2</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -3896,18 +3917,18 @@
         <v>1</v>
       </c>
       <c r="D75" s="2">
-        <v>0.36753000000000002</v>
+        <v>0.30292999999999998</v>
       </c>
       <c r="E75" s="2">
-        <v>0.72040000000000004</v>
+        <v>0.73987999999999998</v>
       </c>
       <c r="F75">
         <f>1-E75</f>
-        <v>0.27959999999999996</v>
+        <v>0.26012000000000002</v>
       </c>
       <c r="G75">
         <f>1-D75</f>
-        <v>0.63246999999999998</v>
+        <v>0.69707000000000008</v>
       </c>
       <c r="H75">
         <f>IF(E75&gt;G75,1,2)</f>
@@ -3919,7 +3940,7 @@
       </c>
       <c r="J75" s="1">
         <f>ABS(G75-E75)</f>
-        <v>8.7930000000000064E-2</v>
+        <v>4.2809999999999904E-2</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -3933,30 +3954,30 @@
         <v>1</v>
       </c>
       <c r="D76" s="2">
-        <v>0.38229000000000002</v>
+        <v>0.29616999999999999</v>
       </c>
       <c r="E76" s="2">
-        <v>0.65668000000000004</v>
+        <v>0.69957999999999998</v>
       </c>
       <c r="F76">
         <f>1-E76</f>
-        <v>0.34331999999999996</v>
+        <v>0.30042000000000002</v>
       </c>
       <c r="G76">
         <f>1-D76</f>
-        <v>0.61770999999999998</v>
+        <v>0.70382999999999996</v>
       </c>
       <c r="H76">
         <f>IF(E76&gt;G76,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I76">
         <f>IF(H76=C76,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J76" s="1">
         <f>ABS(G76-E76)</f>
-        <v>3.897000000000006E-2</v>
+        <v>4.249999999999976E-3</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -3970,18 +3991,18 @@
         <v>1</v>
       </c>
       <c r="D77" s="2">
-        <v>0.27733000000000002</v>
+        <v>0.20999000000000001</v>
       </c>
       <c r="E77" s="2">
-        <v>0.72238000000000002</v>
+        <v>0.74358000000000002</v>
       </c>
       <c r="F77">
         <f>1-E77</f>
-        <v>0.27761999999999998</v>
+        <v>0.25641999999999998</v>
       </c>
       <c r="G77">
         <f>1-D77</f>
-        <v>0.72266999999999992</v>
+        <v>0.79000999999999999</v>
       </c>
       <c r="H77">
         <f>IF(E77&gt;G77,1,2)</f>
@@ -3993,7 +4014,7 @@
       </c>
       <c r="J77" s="1">
         <f>ABS(G77-E77)</f>
-        <v>2.8999999999990145E-4</v>
+        <v>4.6429999999999971E-2</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -4007,18 +4028,18 @@
         <v>1</v>
       </c>
       <c r="D78" s="2">
-        <v>0.36092999999999997</v>
+        <v>0.26789000000000002</v>
       </c>
       <c r="E78" s="2">
-        <v>0.72872999999999999</v>
+        <v>0.80022000000000004</v>
       </c>
       <c r="F78">
         <f>1-E78</f>
-        <v>0.27127000000000001</v>
+        <v>0.19977999999999996</v>
       </c>
       <c r="G78">
         <f>1-D78</f>
-        <v>0.63907000000000003</v>
+        <v>0.73211000000000004</v>
       </c>
       <c r="H78">
         <f>IF(E78&gt;G78,1,2)</f>
@@ -4030,7 +4051,7 @@
       </c>
       <c r="J78" s="1">
         <f>ABS(G78-E78)</f>
-        <v>8.9659999999999962E-2</v>
+        <v>6.8110000000000004E-2</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -4044,18 +4065,18 @@
         <v>1</v>
       </c>
       <c r="D79" s="2">
-        <v>0.29819000000000001</v>
+        <v>0.31091999999999997</v>
       </c>
       <c r="E79" s="2">
-        <v>0.73207999999999995</v>
+        <v>0.72675000000000001</v>
       </c>
       <c r="F79">
         <f>1-E79</f>
-        <v>0.26792000000000005</v>
+        <v>0.27324999999999999</v>
       </c>
       <c r="G79">
         <f>1-D79</f>
-        <v>0.70181000000000004</v>
+        <v>0.68908000000000003</v>
       </c>
       <c r="H79">
         <f>IF(E79&gt;G79,1,2)</f>
@@ -4067,7 +4088,7 @@
       </c>
       <c r="J79" s="1">
         <f>ABS(G79-E79)</f>
-        <v>3.0269999999999908E-2</v>
+        <v>3.7669999999999981E-2</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -4081,18 +4102,18 @@
         <v>2</v>
       </c>
       <c r="D80" s="2">
-        <v>0.28538999999999998</v>
+        <v>0.21359</v>
       </c>
       <c r="E80" s="2">
-        <v>0.68628</v>
+        <v>0.73180999999999996</v>
       </c>
       <c r="F80">
         <f>1-E80</f>
-        <v>0.31372</v>
+        <v>0.26819000000000004</v>
       </c>
       <c r="G80">
         <f>1-D80</f>
-        <v>0.71460999999999997</v>
+        <v>0.78641000000000005</v>
       </c>
       <c r="H80">
         <f>IF(E80&gt;G80,1,2)</f>
@@ -4104,7 +4125,7 @@
       </c>
       <c r="J80" s="1">
         <f>ABS(G80-E80)</f>
-        <v>2.8329999999999966E-2</v>
+        <v>5.4600000000000093E-2</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -4118,18 +4139,18 @@
         <v>1</v>
       </c>
       <c r="D81" s="2">
-        <v>0.39910000000000001</v>
+        <v>0.31941000000000003</v>
       </c>
       <c r="E81" s="2">
-        <v>0.72299000000000002</v>
+        <v>0.71621999999999997</v>
       </c>
       <c r="F81">
         <f>1-E81</f>
-        <v>0.27700999999999998</v>
+        <v>0.28378000000000003</v>
       </c>
       <c r="G81">
         <f>1-D81</f>
-        <v>0.60089999999999999</v>
+        <v>0.68059000000000003</v>
       </c>
       <c r="H81">
         <f>IF(E81&gt;G81,1,2)</f>
@@ -4141,7 +4162,7 @@
       </c>
       <c r="J81" s="1">
         <f>ABS(G81-E81)</f>
-        <v>0.12209000000000003</v>
+        <v>3.5629999999999939E-2</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -4155,18 +4176,18 @@
         <v>2</v>
       </c>
       <c r="D82" s="2">
-        <v>0.27644000000000002</v>
+        <v>0.21709999999999999</v>
       </c>
       <c r="E82" s="2">
-        <v>0.68089</v>
+        <v>0.75202000000000002</v>
       </c>
       <c r="F82">
         <f>1-E82</f>
-        <v>0.31911</v>
+        <v>0.24797999999999998</v>
       </c>
       <c r="G82">
         <f>1-D82</f>
-        <v>0.72355999999999998</v>
+        <v>0.78290000000000004</v>
       </c>
       <c r="H82">
         <f>IF(E82&gt;G82,1,2)</f>
@@ -4178,7 +4199,7 @@
       </c>
       <c r="J82" s="1">
         <f>ABS(G82-E82)</f>
-        <v>4.2669999999999986E-2</v>
+        <v>3.0880000000000019E-2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
@@ -4192,18 +4213,18 @@
         <v>2</v>
       </c>
       <c r="D83" s="2">
-        <v>0.24626999999999999</v>
+        <v>0.20655000000000001</v>
       </c>
       <c r="E83" s="2">
-        <v>0.73604999999999998</v>
+        <v>0.75578999999999996</v>
       </c>
       <c r="F83">
         <f>1-E83</f>
-        <v>0.26395000000000002</v>
+        <v>0.24421000000000004</v>
       </c>
       <c r="G83">
         <f>1-D83</f>
-        <v>0.75373000000000001</v>
+        <v>0.79344999999999999</v>
       </c>
       <c r="H83">
         <f>IF(E83&gt;G83,1,2)</f>
@@ -4215,7 +4236,7 @@
       </c>
       <c r="J83" s="1">
         <f>ABS(G83-E83)</f>
-        <v>1.7680000000000029E-2</v>
+        <v>3.7660000000000027E-2</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
@@ -4229,18 +4250,18 @@
         <v>1</v>
       </c>
       <c r="D84" s="2">
-        <v>0.38246999999999998</v>
+        <v>0.31235000000000002</v>
       </c>
       <c r="E84" s="2">
-        <v>0.74226999999999999</v>
+        <v>0.72380999999999995</v>
       </c>
       <c r="F84">
         <f>1-E84</f>
-        <v>0.25773000000000001</v>
+        <v>0.27619000000000005</v>
       </c>
       <c r="G84">
         <f>1-D84</f>
-        <v>0.61753000000000002</v>
+        <v>0.68764999999999998</v>
       </c>
       <c r="H84">
         <f>IF(E84&gt;G84,1,2)</f>
@@ -4252,7 +4273,7 @@
       </c>
       <c r="J84" s="1">
         <f>ABS(G84-E84)</f>
-        <v>0.12473999999999996</v>
+        <v>3.615999999999997E-2</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
@@ -4266,18 +4287,18 @@
         <v>1</v>
       </c>
       <c r="D85" s="2">
-        <v>0.34798000000000001</v>
+        <v>0.28466999999999998</v>
       </c>
       <c r="E85" s="2">
-        <v>0.74309999999999998</v>
+        <v>0.75139</v>
       </c>
       <c r="F85">
         <f>1-E85</f>
-        <v>0.25690000000000002</v>
+        <v>0.24861</v>
       </c>
       <c r="G85">
         <f>1-D85</f>
-        <v>0.65202000000000004</v>
+        <v>0.71533000000000002</v>
       </c>
       <c r="H85">
         <f>IF(E85&gt;G85,1,2)</f>
@@ -4289,7 +4310,7 @@
       </c>
       <c r="J85" s="1">
         <f>ABS(G85-E85)</f>
-        <v>9.1079999999999939E-2</v>
+        <v>3.6059999999999981E-2</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -4303,18 +4324,18 @@
         <v>1</v>
       </c>
       <c r="D86" s="2">
-        <v>0.39879999999999999</v>
+        <v>0.32095000000000001</v>
       </c>
       <c r="E86" s="2">
-        <v>0.71828000000000003</v>
+        <v>0.72677000000000003</v>
       </c>
       <c r="F86">
         <f>1-E86</f>
-        <v>0.28171999999999997</v>
+        <v>0.27322999999999997</v>
       </c>
       <c r="G86">
         <f>1-D86</f>
-        <v>0.60119999999999996</v>
+        <v>0.67904999999999993</v>
       </c>
       <c r="H86">
         <f>IF(E86&gt;G86,1,2)</f>
@@ -4326,7 +4347,7 @@
       </c>
       <c r="J86" s="1">
         <f>ABS(G86-E86)</f>
-        <v>0.11708000000000007</v>
+        <v>4.7720000000000096E-2</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
@@ -4340,18 +4361,18 @@
         <v>1</v>
       </c>
       <c r="D87" s="2">
-        <v>0.31</v>
+        <v>0.248</v>
       </c>
       <c r="E87" s="2">
-        <v>0.75763000000000003</v>
+        <v>0.75995000000000001</v>
       </c>
       <c r="F87">
         <f>1-E87</f>
-        <v>0.24236999999999997</v>
+        <v>0.24004999999999999</v>
       </c>
       <c r="G87">
         <f>1-D87</f>
-        <v>0.69</v>
+        <v>0.752</v>
       </c>
       <c r="H87">
         <f>IF(E87&gt;G87,1,2)</f>
@@ -4363,7 +4384,7 @@
       </c>
       <c r="J87" s="1">
         <f>ABS(G87-E87)</f>
-        <v>6.7630000000000079E-2</v>
+        <v>7.9500000000000126E-3</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -4377,18 +4398,18 @@
         <v>1</v>
       </c>
       <c r="D88" s="2">
-        <v>0.39572000000000002</v>
+        <v>0.33339999999999997</v>
       </c>
       <c r="E88" s="2">
-        <v>0.71616000000000002</v>
+        <v>0.71336999999999995</v>
       </c>
       <c r="F88">
         <f>1-E88</f>
-        <v>0.28383999999999998</v>
+        <v>0.28663000000000005</v>
       </c>
       <c r="G88">
         <f>1-D88</f>
-        <v>0.60427999999999993</v>
+        <v>0.66660000000000008</v>
       </c>
       <c r="H88">
         <f>IF(E88&gt;G88,1,2)</f>
@@ -4400,7 +4421,7 @@
       </c>
       <c r="J88" s="1">
         <f>ABS(G88-E88)</f>
-        <v>0.11188000000000009</v>
+        <v>4.6769999999999867E-2</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -4414,30 +4435,30 @@
         <v>1</v>
       </c>
       <c r="D89" s="2">
-        <v>0.31935999999999998</v>
+        <v>0.27634999999999998</v>
       </c>
       <c r="E89" s="2">
-        <v>0.73272000000000004</v>
+        <v>0.71945999999999999</v>
       </c>
       <c r="F89">
         <f>1-E89</f>
-        <v>0.26727999999999996</v>
+        <v>0.28054000000000001</v>
       </c>
       <c r="G89">
         <f>1-D89</f>
-        <v>0.68064000000000002</v>
+        <v>0.72365000000000002</v>
       </c>
       <c r="H89">
         <f>IF(E89&gt;G89,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I89">
         <f>IF(H89=C89,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J89" s="1">
         <f>ABS(G89-E89)</f>
-        <v>5.2080000000000015E-2</v>
+        <v>4.190000000000027E-3</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
@@ -4451,18 +4472,18 @@
         <v>1</v>
       </c>
       <c r="D90" s="2">
-        <v>0.34893999999999997</v>
+        <v>0.31407000000000002</v>
       </c>
       <c r="E90" s="2">
-        <v>0.76439000000000001</v>
+        <v>0.75566999999999995</v>
       </c>
       <c r="F90">
         <f>1-E90</f>
-        <v>0.23560999999999999</v>
+        <v>0.24433000000000005</v>
       </c>
       <c r="G90">
         <f>1-D90</f>
-        <v>0.65105999999999997</v>
+        <v>0.68592999999999993</v>
       </c>
       <c r="H90">
         <f>IF(E90&gt;G90,1,2)</f>
@@ -4474,7 +4495,7 @@
       </c>
       <c r="J90" s="1">
         <f>ABS(G90-E90)</f>
-        <v>0.11333000000000004</v>
+        <v>6.9740000000000024E-2</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -4488,18 +4509,18 @@
         <v>1</v>
       </c>
       <c r="D91" s="2">
-        <v>0.36188999999999999</v>
+        <v>0.33556000000000002</v>
       </c>
       <c r="E91" s="2">
-        <v>0.72660000000000002</v>
+        <v>0.67949000000000004</v>
       </c>
       <c r="F91">
         <f>1-E91</f>
-        <v>0.27339999999999998</v>
+        <v>0.32050999999999996</v>
       </c>
       <c r="G91">
         <f>1-D91</f>
-        <v>0.63810999999999996</v>
+        <v>0.66443999999999992</v>
       </c>
       <c r="H91">
         <f>IF(E91&gt;G91,1,2)</f>
@@ -4511,7 +4532,7 @@
       </c>
       <c r="J91" s="1">
         <f>ABS(G91-E91)</f>
-        <v>8.8490000000000069E-2</v>
+        <v>1.5050000000000119E-2</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -4525,18 +4546,18 @@
         <v>2</v>
       </c>
       <c r="D92" s="2">
-        <v>0.37141000000000002</v>
+        <v>0.35333999999999999</v>
       </c>
       <c r="E92" s="2">
-        <v>0.68669000000000002</v>
+        <v>0.65756000000000003</v>
       </c>
       <c r="F92">
         <f>1-E92</f>
-        <v>0.31330999999999998</v>
+        <v>0.34243999999999997</v>
       </c>
       <c r="G92">
         <f>1-D92</f>
-        <v>0.62858999999999998</v>
+        <v>0.64666000000000001</v>
       </c>
       <c r="H92">
         <f>IF(E92&gt;G92,1,2)</f>
@@ -4548,7 +4569,7 @@
       </c>
       <c r="J92" s="1">
         <f>ABS(G92-E92)</f>
-        <v>5.8100000000000041E-2</v>
+        <v>1.0900000000000021E-2</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -4562,18 +4583,18 @@
         <v>1</v>
       </c>
       <c r="D93" s="2">
-        <v>0.31435999999999997</v>
+        <v>0.34641</v>
       </c>
       <c r="E93" s="2">
-        <v>0.70015000000000005</v>
+        <v>0.68798999999999999</v>
       </c>
       <c r="F93">
         <f>1-E93</f>
-        <v>0.29984999999999995</v>
+        <v>0.31201000000000001</v>
       </c>
       <c r="G93">
         <f>1-D93</f>
-        <v>0.68564000000000003</v>
+        <v>0.65359</v>
       </c>
       <c r="H93">
         <f>IF(E93&gt;G93,1,2)</f>
@@ -4585,7 +4606,7 @@
       </c>
       <c r="J93" s="1">
         <f>ABS(G93-E93)</f>
-        <v>1.4510000000000023E-2</v>
+        <v>3.4399999999999986E-2</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -4599,30 +4620,30 @@
         <v>2</v>
       </c>
       <c r="D94" s="2">
-        <v>0.29310000000000003</v>
+        <v>0.27771000000000001</v>
       </c>
       <c r="E94" s="2">
-        <v>0.69459000000000004</v>
+        <v>0.73070000000000002</v>
       </c>
       <c r="F94">
         <f>1-E94</f>
-        <v>0.30540999999999996</v>
+        <v>0.26929999999999998</v>
       </c>
       <c r="G94">
         <f>1-D94</f>
-        <v>0.70689999999999997</v>
+        <v>0.72228999999999999</v>
       </c>
       <c r="H94">
         <f>IF(E94&gt;G94,1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I94">
         <f>IF(H94=C94,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J94" s="1">
         <f>ABS(G94-E94)</f>
-        <v>1.2309999999999932E-2</v>
+        <v>8.4100000000000286E-3</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
@@ -4636,30 +4657,30 @@
         <v>1</v>
       </c>
       <c r="D95" s="2">
-        <v>0.33310000000000001</v>
+        <v>0.28117999999999999</v>
       </c>
       <c r="E95" s="2">
-        <v>0.76254999999999995</v>
+        <v>0.69259999999999999</v>
       </c>
       <c r="F95">
         <f>1-E95</f>
-        <v>0.23745000000000005</v>
+        <v>0.30740000000000001</v>
       </c>
       <c r="G95">
         <f>1-D95</f>
-        <v>0.66690000000000005</v>
+        <v>0.71882000000000001</v>
       </c>
       <c r="H95">
         <f>IF(E95&gt;G95,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I95">
         <f>IF(H95=C95,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J95" s="1">
         <f>ABS(G95-E95)</f>
-        <v>9.5649999999999902E-2</v>
+        <v>2.6220000000000021E-2</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -4673,18 +4694,18 @@
         <v>1</v>
       </c>
       <c r="D96" s="2">
-        <v>0.38373000000000002</v>
+        <v>0.35779</v>
       </c>
       <c r="E96" s="2">
-        <v>0.73282999999999998</v>
+        <v>0.69233</v>
       </c>
       <c r="F96">
         <f>1-E96</f>
-        <v>0.26717000000000002</v>
+        <v>0.30767</v>
       </c>
       <c r="G96">
         <f>1-D96</f>
-        <v>0.61626999999999998</v>
+        <v>0.64220999999999995</v>
       </c>
       <c r="H96">
         <f>IF(E96&gt;G96,1,2)</f>
@@ -4696,7 +4717,7 @@
       </c>
       <c r="J96" s="1">
         <f>ABS(G96-E96)</f>
-        <v>0.11656</v>
+        <v>5.0120000000000053E-2</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
@@ -4710,18 +4731,18 @@
         <v>1</v>
       </c>
       <c r="D97" s="2">
-        <v>0.31381999999999999</v>
+        <v>0.33539999999999998</v>
       </c>
       <c r="E97" s="2">
-        <v>0.76502999999999999</v>
+        <v>0.71128999999999998</v>
       </c>
       <c r="F97">
         <f>1-E97</f>
-        <v>0.23497000000000001</v>
+        <v>0.28871000000000002</v>
       </c>
       <c r="G97">
         <f>1-D97</f>
-        <v>0.68618000000000001</v>
+        <v>0.66460000000000008</v>
       </c>
       <c r="H97">
         <f>IF(E97&gt;G97,1,2)</f>
@@ -4733,7 +4754,7 @@
       </c>
       <c r="J97" s="1">
         <f>ABS(G97-E97)</f>
-        <v>7.8849999999999976E-2</v>
+        <v>4.6689999999999898E-2</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
@@ -4747,18 +4768,18 @@
         <v>1</v>
       </c>
       <c r="D98" s="2">
-        <v>0.41781000000000001</v>
+        <v>0.35672999999999999</v>
       </c>
       <c r="E98" s="2">
-        <v>0.74634999999999996</v>
+        <v>0.73036000000000001</v>
       </c>
       <c r="F98">
         <f>1-E98</f>
-        <v>0.25365000000000004</v>
+        <v>0.26963999999999999</v>
       </c>
       <c r="G98">
         <f>1-D98</f>
-        <v>0.58218999999999999</v>
+        <v>0.64327000000000001</v>
       </c>
       <c r="H98">
         <f>IF(E98&gt;G98,1,2)</f>
@@ -4770,7 +4791,7 @@
       </c>
       <c r="J98" s="1">
         <f>ABS(G98-E98)</f>
-        <v>0.16415999999999997</v>
+        <v>8.7090000000000001E-2</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
@@ -4784,18 +4805,18 @@
         <v>2</v>
       </c>
       <c r="D99" s="2">
-        <v>0.2296</v>
+        <v>0.24223</v>
       </c>
       <c r="E99" s="2">
-        <v>0.78902000000000005</v>
+        <v>0.81679999999999997</v>
       </c>
       <c r="F99">
         <f>1-E99</f>
-        <v>0.21097999999999995</v>
+        <v>0.18320000000000003</v>
       </c>
       <c r="G99">
         <f>1-D99</f>
-        <v>0.77039999999999997</v>
+        <v>0.75777000000000005</v>
       </c>
       <c r="H99">
         <f>IF(E99&gt;G99,1,2)</f>
@@ -4807,7 +4828,7 @@
       </c>
       <c r="J99" s="1">
         <f>ABS(G99-E99)</f>
-        <v>1.8620000000000081E-2</v>
+        <v>5.9029999999999916E-2</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
@@ -4821,18 +4842,18 @@
         <v>1</v>
       </c>
       <c r="D100" s="2">
-        <v>0.35471000000000003</v>
+        <v>0.33396999999999999</v>
       </c>
       <c r="E100" s="2">
-        <v>0.78974</v>
+        <v>0.77481999999999995</v>
       </c>
       <c r="F100">
         <f>1-E100</f>
-        <v>0.21026</v>
+        <v>0.22518000000000005</v>
       </c>
       <c r="G100">
         <f>1-D100</f>
-        <v>0.64528999999999992</v>
+        <v>0.66603000000000001</v>
       </c>
       <c r="H100">
         <f>IF(E100&gt;G100,1,2)</f>
@@ -4844,7 +4865,7 @@
       </c>
       <c r="J100" s="1">
         <f>ABS(G100-E100)</f>
-        <v>0.14445000000000008</v>
+        <v>0.10878999999999994</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
@@ -4858,30 +4879,30 @@
         <v>1</v>
       </c>
       <c r="D101" s="2">
-        <v>0.25146000000000002</v>
+        <v>0.20677999999999999</v>
       </c>
       <c r="E101" s="2">
-        <v>0.75044</v>
+        <v>0.77246999999999999</v>
       </c>
       <c r="F101">
         <f>1-E101</f>
-        <v>0.24956</v>
+        <v>0.22753000000000001</v>
       </c>
       <c r="G101">
         <f>1-D101</f>
-        <v>0.74853999999999998</v>
+        <v>0.79322000000000004</v>
       </c>
       <c r="H101">
         <f>IF(E101&gt;G101,1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I101">
         <f>IF(H101=C101,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J101" s="1">
         <f>ABS(G101-E101)</f>
-        <v>1.9000000000000128E-3</v>
+        <v>2.0750000000000046E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>